<commit_message>
atualização de ativadade antiga, base de dados e inicio do mundo 2 em Python
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projetos\PycharmProjects\AutomateInstagram\AutomatinoIG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC3635D-47AD-4F3C-94A3-1BC025D29228}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C62508A-1827-4A03-91C1-60145788CB33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16857,7 +16857,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5486"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -44335,10 +44337,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B5327C2-A79D-405A-BCC2-6A3BF07D19DD}">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A11"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44355,46 +44357,71 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>95</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>120</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>135</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>203</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>374</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>407</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>500</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>600</v>
+        <v>374</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>900</v>
       </c>
     </row>

</xml_diff>